<commit_message>
Refactored combat to make it more flexible. Some debugging.
</commit_message>
<xml_diff>
--- a/de.rauwolf.gaming.battleships/resources/ArmorExampleCalcs.xlsx
+++ b/de.rauwolf.gaming.battleships/resources/ArmorExampleCalcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr showObjects="none" filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="405" windowWidth="14805" windowHeight="7710"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Avg. Damage vs. Target" sheetId="3" r:id="rId1"/>
@@ -256,9 +256,6 @@
     <t>'Sadist' Particle Beam</t>
   </si>
   <si>
-    <t>Locks on Target till destroyed or shields back up again. Cannot penetrate Shields. Will only ever fire at unshielded targets.</t>
-  </si>
-  <si>
     <t>'Thunderstorm' Arc Thrower</t>
   </si>
   <si>
@@ -365,6 +362,9 @@
   </si>
   <si>
     <t>Monstrosity' Siege Artillery</t>
+  </si>
+  <si>
+    <t>-50% Shield Pierce</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1442,6 +1442,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1747,10 +1750,10 @@
   <dimension ref="A1:U99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="8" topLeftCell="M30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="8" topLeftCell="L21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,7 +1791,7 @@
         <v>43</v>
       </c>
       <c r="E1" s="103" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="1"/>
@@ -1836,7 +1839,7 @@
         <v>5</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>6</v>
@@ -2068,7 +2071,7 @@
       <c r="T5" s="101"/>
       <c r="U5" s="102">
         <f>AVERAGE(R9:R100)</f>
-        <v>17.567129629629626</v>
+        <v>19.194467592592588</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="68" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3119,7 +3122,7 @@
         <v>95.555555555555557</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>77</v>
       </c>
@@ -3130,14 +3133,14 @@
         <v>68</v>
       </c>
       <c r="D21" s="38">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E21" s="38">
         <v>1</v>
       </c>
       <c r="F21" s="39">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G21" s="40">
         <v>50</v>
@@ -3148,58 +3151,58 @@
       <c r="I21" s="42" t="str">
         <f t="shared" si="4"/>
         <v>30*(0/0/100)
---&gt; 30,0%, avg.  1,35</v>
+--&gt; 30,0%, avg.  3,6</v>
       </c>
       <c r="J21" s="42" t="str">
         <f t="shared" si="4"/>
         <v>50*(0/0/100)
---&gt; 50,0%, avg.  2,25</v>
+--&gt; 50,0%, avg.  6,0</v>
       </c>
       <c r="K21" s="42" t="str">
         <f t="shared" si="4"/>
         <v>70*(0/0/100)
---&gt; 70,0%, avg.  3,15</v>
+--&gt; 70,0%, avg.  8,4</v>
       </c>
       <c r="L21" s="42" t="str">
         <f t="shared" si="4"/>
         <v>85*(0/0/100)
---&gt; 85,0%, avg.  3,83</v>
+--&gt; 85,0%, avg.  10,2</v>
       </c>
       <c r="M21" s="42" t="str">
         <f t="shared" si="4"/>
         <v>100*(0/0/100)
---&gt; 100,0%, avg.  4,5</v>
+--&gt; 100,0%, avg.  12,0</v>
       </c>
       <c r="N21" s="42" t="str">
         <f t="shared" si="4"/>
         <v>100*(0/0/100)
---&gt; 100,0%, avg.  4,5</v>
+--&gt; 100,0%, avg.  12,0</v>
       </c>
       <c r="O21" s="42" t="str">
         <f t="shared" si="4"/>
         <v>100*(0/0/100)
---&gt; 100,0%, avg.  4,5</v>
+--&gt; 100,0%, avg.  12,0</v>
       </c>
       <c r="P21" s="42" t="str">
         <f t="shared" si="4"/>
         <v>100*(0/10/90)
---&gt; 100,0%, avg.  4,35</v>
+--&gt; 100,0%, avg.  11,6</v>
       </c>
       <c r="Q21" s="42" t="str">
         <f t="shared" si="4"/>
         <v>100*(0/50/50)
---&gt; 100,0%, avg.  3,75</v>
+--&gt; 100,0%, avg.  10,0</v>
       </c>
       <c r="R21" s="36">
         <f t="shared" si="2"/>
-        <v>3.5755555555555554</v>
+        <v>9.5333333333333332</v>
       </c>
       <c r="S21" s="54">
         <f t="shared" si="3"/>
         <v>81.666666666666671</v>
       </c>
-      <c r="T21" s="55" t="s">
-        <v>78</v>
+      <c r="T21" s="110" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -3743,20 +3746,20 @@
         <v>69</v>
       </c>
       <c r="D29" s="38">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="E29" s="38">
         <v>50</v>
       </c>
       <c r="F29" s="39">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G29" s="40">
         <v>0</v>
       </c>
       <c r="H29" s="41">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="I29" s="42" t="str">
         <f t="shared" si="6"/>
@@ -3771,41 +3774,41 @@
       <c r="K29" s="42" t="str">
         <f t="shared" si="6"/>
         <v>20*(0/0/100)
---&gt; 20,0%, avg.  7,2</v>
+--&gt; 20,0%, avg.  5,4</v>
       </c>
       <c r="L29" s="42" t="str">
         <f t="shared" si="6"/>
-        <v>35*(0/10/90)
---&gt; 35,0%, avg.  12,18</v>
+        <v>35*(0/0/100)
+--&gt; 35,0%, avg.  9,45</v>
       </c>
       <c r="M29" s="42" t="str">
         <f t="shared" si="6"/>
-        <v>50*(0/25/75)
---&gt; 50,0%, avg.  16,5</v>
+        <v>50*(0/5/95)
+--&gt; 50,0%, avg.  13,28</v>
       </c>
       <c r="N29" s="42" t="str">
         <f t="shared" si="6"/>
-        <v>60*(0/30/70)
---&gt; 60,0%, avg.  19,44</v>
+        <v>60*(0/10/90)
+--&gt; 60,0%, avg.  15,66</v>
       </c>
       <c r="O29" s="42" t="str">
         <f t="shared" si="6"/>
-        <v>70*(5/45/50)
---&gt; 70,0%, avg.  20,45</v>
+        <v>70*(0/30/70)
+--&gt; 70,0%, avg.  17,01</v>
       </c>
       <c r="P29" s="42" t="str">
         <f t="shared" si="6"/>
-        <v>90*(20/40/40)
---&gt; 90,0%, avg.  23,11</v>
+        <v>90*(0/40/60)
+--&gt; 90,0%, avg.  21,06</v>
       </c>
       <c r="Q29" s="42" t="str">
         <f t="shared" si="6"/>
-        <v>100*(50/50/0)
---&gt; 100,0%, avg.  16,2</v>
+        <v>100*(30/50/20)
+--&gt; 100,0%, avg.  16,29</v>
       </c>
       <c r="R29" s="36">
         <f t="shared" si="2"/>
-        <v>12.786666666666667</v>
+        <v>10.905555555555557</v>
       </c>
       <c r="S29" s="54">
         <f t="shared" si="3"/>
@@ -3997,7 +4000,7 @@
     </row>
     <row r="33" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B33" s="43" t="s">
         <v>46</v>
@@ -4246,14 +4249,14 @@
         <v>70</v>
       </c>
       <c r="D36" s="38">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="E36" s="38">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F36" s="39">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="G36" s="40">
         <v>20</v>
@@ -4269,46 +4272,46 @@
       <c r="J36" s="42" t="str">
         <f t="shared" si="6"/>
         <v>20*(0/0/100)
---&gt; 20,0%, avg.  7,2</v>
+--&gt; 20,0%, avg.  10,0</v>
       </c>
       <c r="K36" s="42" t="str">
         <f t="shared" si="6"/>
         <v>40*(0/0/100)
---&gt; 40,0%, avg.  14,4</v>
+--&gt; 40,0%, avg.  20,0</v>
       </c>
       <c r="L36" s="42" t="str">
         <f t="shared" si="6"/>
         <v>55*(0/10/90)
---&gt; 55,0%, avg.  19,14</v>
+--&gt; 55,0%, avg.  26,58</v>
       </c>
       <c r="M36" s="42" t="str">
         <f t="shared" si="6"/>
         <v>70*(0/25/75)
---&gt; 70,0%, avg.  23,1</v>
+--&gt; 70,0%, avg.  32,08</v>
       </c>
       <c r="N36" s="42" t="str">
         <f t="shared" si="6"/>
         <v>80*(0/30/70)
---&gt; 80,0%, avg.  25,92</v>
+--&gt; 80,0%, avg.  36,0</v>
       </c>
       <c r="O36" s="42" t="str">
         <f t="shared" si="6"/>
         <v>90*(5/45/50)
---&gt; 90,0%, avg.  26,3</v>
+--&gt; 90,0%, avg.  36,53</v>
       </c>
       <c r="P36" s="42" t="str">
         <f t="shared" si="6"/>
         <v>100*(20/40/40)
---&gt; 100,0%, avg.  25,68</v>
+--&gt; 100,0%, avg.  35,67</v>
       </c>
       <c r="Q36" s="42" t="str">
         <f t="shared" si="6"/>
         <v>100*(50/50/0)
---&gt; 100,0%, avg.  16,2</v>
+--&gt; 100,0%, avg.  22,5</v>
       </c>
       <c r="R36" s="36">
         <f t="shared" si="2"/>
-        <v>17.548888888888889</v>
+        <v>24.373333333333335</v>
       </c>
       <c r="S36" s="54">
         <f t="shared" si="3"/>
@@ -4477,7 +4480,7 @@
     </row>
     <row r="39" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" s="43" t="s">
         <v>46</v>
@@ -5137,7 +5140,7 @@
     </row>
     <row r="48" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B48" s="43" t="s">
         <v>47</v>
@@ -5326,20 +5329,20 @@
         <v>69</v>
       </c>
       <c r="D51" s="38">
-        <v>10000</v>
+        <v>200</v>
       </c>
       <c r="E51" s="38">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F51" s="39">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G51" s="40">
         <v>0</v>
       </c>
       <c r="H51" s="41">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="I51" s="42" t="str">
         <f t="shared" si="10"/>
@@ -5354,125 +5357,125 @@
       <c r="K51" s="42" t="str">
         <f t="shared" si="10"/>
         <v>20*(0/0/100)
---&gt; 20,0%, avg.  30,0</v>
+--&gt; 20,0%, avg.  60,0</v>
       </c>
       <c r="L51" s="42" t="str">
         <f t="shared" si="10"/>
-        <v>35*(0/0/100)
---&gt; 35,0%, avg.  52,5</v>
+        <v>35*(0/10/90)
+--&gt; 35,0%, avg.  101,5</v>
       </c>
       <c r="M51" s="42" t="str">
+        <f t="shared" si="10"/>
+        <v>50*(0/25/75)
+--&gt; 50,0%, avg.  137,5</v>
+      </c>
+      <c r="N51" s="42" t="str">
+        <f t="shared" si="10"/>
+        <v>60*(0/30/70)
+--&gt; 60,0%, avg.  162,0</v>
+      </c>
+      <c r="O51" s="42" t="str">
+        <f t="shared" si="10"/>
+        <v>70*(5/45/50)
+--&gt; 70,0%, avg.  170,45</v>
+      </c>
+      <c r="P51" s="42" t="str">
+        <f t="shared" si="10"/>
+        <v>90*(20/40/40)
+--&gt; 90,0%, avg.  192,6</v>
+      </c>
+      <c r="Q51" s="42" t="str">
+        <f t="shared" si="10"/>
+        <v>100*(50/50/0)
+--&gt; 100,0%, avg.  135,0</v>
+      </c>
+      <c r="R51" s="36">
+        <f t="shared" si="2"/>
+        <v>106.56111111111112</v>
+      </c>
+      <c r="S51" s="54">
+        <f t="shared" si="9"/>
+        <v>47.222222222222221</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="38">
+        <v>10000</v>
+      </c>
+      <c r="E52" s="38">
+        <v>100</v>
+      </c>
+      <c r="F52" s="39">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="G52" s="40">
+        <v>30</v>
+      </c>
+      <c r="H52" s="41">
+        <v>1000</v>
+      </c>
+      <c r="I52" s="42" t="str">
+        <f t="shared" si="10"/>
+        <v>10*(0/0/100)
+--&gt; 10,0%, avg.  15,0</v>
+      </c>
+      <c r="J52" s="42" t="str">
+        <f t="shared" si="10"/>
+        <v>30*(0/0/100)
+--&gt; 30,0%, avg.  45,0</v>
+      </c>
+      <c r="K52" s="42" t="str">
         <f t="shared" si="10"/>
         <v>50*(0/0/100)
 --&gt; 50,0%, avg.  75,0</v>
       </c>
-      <c r="N51" s="42" t="str">
+      <c r="L52" s="42" t="str">
         <f t="shared" si="10"/>
-        <v>60*(0/0/100)
---&gt; 60,0%, avg.  90,0</v>
-      </c>
-      <c r="O51" s="42" t="str">
+        <v>65*(0/0/100)
+--&gt; 65,0%, avg.  97,5</v>
+      </c>
+      <c r="M52" s="42" t="str">
         <f t="shared" si="10"/>
-        <v>70*(0/0/100)
---&gt; 70,0%, avg.  105,0</v>
-      </c>
-      <c r="P51" s="42" t="str">
+        <v>80*(0/0/100)
+--&gt; 80,0%, avg.  120,0</v>
+      </c>
+      <c r="N52" s="42" t="str">
         <f t="shared" si="10"/>
         <v>90*(0/0/100)
 --&gt; 90,0%, avg.  135,0</v>
       </c>
-      <c r="Q51" s="42" t="str">
+      <c r="O52" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(0/0/100)
 --&gt; 100,0%, avg.  150,0</v>
       </c>
-      <c r="R51" s="36">
-        <f t="shared" si="2"/>
-        <v>70.833333333333329</v>
-      </c>
-      <c r="S51" s="54">
-        <f t="shared" si="9"/>
-        <v>47.222222222222221</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" s="38">
-        <v>80</v>
-      </c>
-      <c r="E52" s="38">
-        <v>1</v>
-      </c>
-      <c r="F52" s="39">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="G52" s="40">
-        <v>50</v>
-      </c>
-      <c r="H52" s="41">
-        <v>100</v>
-      </c>
-      <c r="I52" s="42" t="str">
-        <f t="shared" si="10"/>
-        <v>30*(0/0/100)
---&gt; 30,0%, avg.  36,0</v>
-      </c>
-      <c r="J52" s="42" t="str">
-        <f t="shared" si="10"/>
-        <v>50*(0/0/100)
---&gt; 50,0%, avg.  60,0</v>
-      </c>
-      <c r="K52" s="42" t="str">
-        <f t="shared" si="10"/>
-        <v>70*(0/0/100)
---&gt; 70,0%, avg.  84,0</v>
-      </c>
-      <c r="L52" s="42" t="str">
-        <f t="shared" si="10"/>
-        <v>85*(0/10/90)
---&gt; 85,0%, avg.  98,6</v>
-      </c>
-      <c r="M52" s="42" t="str">
-        <f t="shared" si="10"/>
-        <v>100*(0/25/75)
---&gt; 100,0%, avg.  110,0</v>
-      </c>
-      <c r="N52" s="42" t="str">
-        <f t="shared" si="10"/>
-        <v>100*(0/30/70)
---&gt; 100,0%, avg.  108,0</v>
-      </c>
-      <c r="O52" s="42" t="str">
-        <f t="shared" si="10"/>
-        <v>100*(5/45/50)
---&gt; 100,0%, avg.  97,4</v>
-      </c>
       <c r="P52" s="42" t="str">
         <f t="shared" si="10"/>
-        <v>100*(20/40/40)
---&gt; 100,0%, avg.  85,6</v>
+        <v>100*(0/0/100)
+--&gt; 100,0%, avg.  150,0</v>
       </c>
       <c r="Q52" s="42" t="str">
         <f t="shared" si="10"/>
-        <v>100*(50/50/0)
---&gt; 100,0%, avg.  54,0</v>
+        <v>100*(0/0/100)
+--&gt; 100,0%, avg.  150,0</v>
       </c>
       <c r="R52" s="36">
         <f t="shared" si="2"/>
-        <v>81.51111111111112</v>
+        <v>104.16666666666667</v>
       </c>
       <c r="S52" s="54">
         <f t="shared" si="9"/>
-        <v>81.666666666666671</v>
+        <v>69.444444444444443</v>
       </c>
       <c r="T52" s="55" t="s">
         <v>59</v>
@@ -5489,17 +5492,17 @@
         <v>69</v>
       </c>
       <c r="D53" s="38">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="E53" s="38">
         <v>1</v>
       </c>
       <c r="F53" s="39">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="G53" s="40">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="H53" s="41">
         <v>0</v>
@@ -5507,51 +5510,51 @@
       <c r="I53" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(20/40/40)
---&gt; 100,0%, avg.  224,7</v>
+--&gt; 100,0%, avg.  246,1</v>
       </c>
       <c r="J53" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(30/40/20)
---&gt; 90,0%, avg.  169,05</v>
+--&gt; 90,0%, avg.  185,15</v>
       </c>
       <c r="K53" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(40/45/0)
---&gt; 85,0%, avg.  123,9</v>
+--&gt; 85,0%, avg.  135,7</v>
       </c>
       <c r="L53" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(40/35/0)
---&gt; 75,0%, avg.  102,9</v>
+--&gt; 75,0%, avg.  112,7</v>
       </c>
       <c r="M53" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(45/20/0)
---&gt; 65,0%, avg.  75,08</v>
+--&gt; 65,0%, avg.  82,23</v>
       </c>
       <c r="N53" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(50/10/0)
---&gt; 60,0%, avg.  57,75</v>
+--&gt; 60,0%, avg.  63,25</v>
       </c>
       <c r="O53" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(50/0/0)
---&gt; 50,0%, avg.  36,75</v>
+--&gt; 50,0%, avg.  40,25</v>
       </c>
       <c r="P53" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(40/0/0)
---&gt; 40,0%, avg.  29,4</v>
+--&gt; 40,0%, avg.  32,2</v>
       </c>
       <c r="Q53" s="42" t="str">
         <f t="shared" si="10"/>
         <v>100*(20/0/0)
---&gt; 20,0%, avg.  14,7</v>
+--&gt; 20,0%, avg.  16,1</v>
       </c>
       <c r="R53" s="36">
         <f t="shared" si="2"/>
-        <v>92.692222222222227</v>
+        <v>101.52000000000002</v>
       </c>
       <c r="S53" s="54">
         <f t="shared" si="9"/>
@@ -5560,7 +5563,7 @@
     </row>
     <row r="54" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B54" s="43" t="s">
         <v>51</v>
@@ -8295,25 +8298,25 @@
         <v>66</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="E1" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>49</v>
@@ -8321,7 +8324,7 @@
     </row>
     <row r="2" spans="1:9" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="88">
         <v>10</v>
@@ -8336,7 +8339,7 @@
         <v>-10</v>
       </c>
       <c r="F2" s="88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" s="88"/>
       <c r="H2" s="88">
@@ -8346,7 +8349,7 @@
     </row>
     <row r="3" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="91">
         <v>0</v>
@@ -8361,7 +8364,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" s="91"/>
       <c r="H3" s="91">
@@ -8371,7 +8374,7 @@
     </row>
     <row r="4" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="91">
         <v>-10</v>
@@ -8386,7 +8389,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="91"/>
       <c r="H4" s="91">
@@ -8396,7 +8399,7 @@
     </row>
     <row r="5" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="91">
         <v>20</v>
@@ -8411,7 +8414,7 @@
         <v>-10</v>
       </c>
       <c r="F5" s="91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="91"/>
       <c r="H5" s="91">
@@ -8421,7 +8424,7 @@
     </row>
     <row r="6" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="91">
         <v>10</v>
@@ -8436,7 +8439,7 @@
         <v>-10</v>
       </c>
       <c r="F6" s="91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" s="91"/>
       <c r="H6" s="91">
@@ -8446,7 +8449,7 @@
     </row>
     <row r="7" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="91">
         <v>5</v>
@@ -8461,7 +8464,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G7" s="91"/>
       <c r="H7" s="91">
@@ -8471,7 +8474,7 @@
     </row>
     <row r="8" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="91">
         <v>0</v>
@@ -8486,7 +8489,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="91"/>
       <c r="H8" s="91">
@@ -8496,7 +8499,7 @@
     </row>
     <row r="9" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="90" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="91">
         <v>0</v>
@@ -8511,7 +8514,7 @@
         <v>-5</v>
       </c>
       <c r="F9" s="91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G9" s="91"/>
       <c r="H9" s="91">
@@ -8521,7 +8524,7 @@
     </row>
     <row r="10" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="91">
         <v>0</v>
@@ -8536,7 +8539,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G10" s="91"/>
       <c r="H10" s="91">
@@ -8546,7 +8549,7 @@
     </row>
     <row r="11" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="91">
         <v>0</v>
@@ -8561,7 +8564,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" s="91"/>
       <c r="H11" s="91">
@@ -8571,7 +8574,7 @@
     </row>
     <row r="12" spans="1:9" s="44" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="91">
         <v>0</v>
@@ -8586,19 +8589,19 @@
         <v>0</v>
       </c>
       <c r="F12" s="91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="91"/>
       <c r="H12" s="91">
         <v>0</v>
       </c>
       <c r="I12" s="92" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="90" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="91">
         <v>-10</v>
@@ -8613,7 +8616,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" s="91"/>
       <c r="H13" s="91">
@@ -8623,7 +8626,7 @@
     </row>
     <row r="14" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="91">
         <v>50</v>
@@ -8638,7 +8641,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G14" s="106" t="s">
         <v>69</v>
@@ -8870,19 +8873,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="64" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="64" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="64" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="E1" s="64" t="s">
         <v>102</v>
-      </c>
-      <c r="E1" s="64" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8972,7 +8975,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="98" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7">
         <v>40</v>

</xml_diff>

<commit_message>
Major performance improvement, some renaming
</commit_message>
<xml_diff>
--- a/de.rauwolf.gaming.battleships/resources/ArmorExampleCalcs.xlsx
+++ b/de.rauwolf.gaming.battleships/resources/ArmorExampleCalcs.xlsx
@@ -1434,6 +1434,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1442,9 +1445,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1750,10 +1750,10 @@
   <dimension ref="A1:U99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="8" topLeftCell="L21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="8" topLeftCell="I9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,17 +1796,17 @@
       <c r="F1" s="2"/>
       <c r="G1" s="1"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="107" t="s">
+      <c r="I1" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
     </row>
     <row r="2" spans="1:21" s="71" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -2127,16 +2127,16 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="68" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="108" t="s">
+      <c r="A7" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="108"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="109"/>
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="110"/>
       <c r="I7" s="23"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
@@ -3201,7 +3201,7 @@
         <f t="shared" si="3"/>
         <v>81.666666666666671</v>
       </c>
-      <c r="T21" s="110" t="s">
+      <c r="T21" s="107" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>